<commit_message>
update image and video link
</commit_message>
<xml_diff>
--- a/cnn_inference_trained.xlsx
+++ b/cnn_inference_trained.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scottreed/PycharmProjects/pharmacogenomics_training/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scottreed/PycharmProjects/Tetris_CNN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FAC3730-6ABE-8F44-8C94-1D845BB2AE64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED69FF6-9EDA-E747-AC3B-1FACF53D5878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -503,7 +503,7 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D35" sqref="B33:D35"/>
+      <selection activeCell="D20" sqref="B18:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -874,7 +874,7 @@
       </c>
       <c r="B1" s="1" t="str">
         <f>INDEX({"Slinky Snake","Bubble Block","Topsy Turvy","Slippery Slide","Zany Zigzag","Jolly Jumper","Lively L"},MATCH(MAX(Softmax!A2:G2),Softmax!A2:G2,0))</f>
-        <v>Lively L</v>
+        <v>Slippery Slide</v>
       </c>
     </row>
   </sheetData>
@@ -916,7 +916,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -939,10 +939,10 @@
       <c r="B2">
         <v>0</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2" s="8">
+      <c r="C2" s="5">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5">
         <v>1</v>
       </c>
     </row>
@@ -950,14 +950,14 @@
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="8">
-        <v>1</v>
-      </c>
-      <c r="C3" s="8">
-        <v>1</v>
-      </c>
-      <c r="D3" s="8">
-        <v>1</v>
+      <c r="B3" s="5">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -995,7 +995,7 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <f>SUMPRODUCT(Inference!B2:C3, Filter!A1:B2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <f>SUMPRODUCT(Inference!C2:D3, Filter!A1:B2)</f>
@@ -1009,7 +1009,7 @@
       </c>
       <c r="B3">
         <f>SUMPRODUCT(Inference!C3:D4, Filter!A1:B2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1033,7 +1033,7 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <f>MAX(0, Conv!A2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <f>MAX(0, Conv!B2)</f>
@@ -1047,7 +1047,7 @@
       </c>
       <c r="B3">
         <f>MAX(0, Conv!B3)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1071,7 +1071,7 @@
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2">
         <f>ReLU!A2</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
@@ -1089,7 +1089,7 @@
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5">
         <f>ReLU!B3</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1241,31 +1241,31 @@
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <f>SUMPRODUCT(Flatten!A2:A5, DenseParameters!A1:A4) + DenseParameters!A6</f>
-        <v>0.73865073919296353</v>
+        <v>2.7920037508010869</v>
       </c>
       <c r="B2">
         <f>SUMPRODUCT(Flatten!A2:A5, DenseParameters!B1:B4) + DenseParameters!B6</f>
-        <v>-9.7328115701675415</v>
+        <v>-0.56554305553436324</v>
       </c>
       <c r="C2">
         <f>SUMPRODUCT(Flatten!A2:A5, DenseParameters!C1:C4) + DenseParameters!C6</f>
-        <v>5.985853910446167</v>
+        <v>2.9987877607345581</v>
       </c>
       <c r="D2">
         <f>SUMPRODUCT(Flatten!A2:A5, DenseParameters!D1:D4) + DenseParameters!D6</f>
-        <v>1.7724983766675013</v>
+        <v>6.8336683660745638</v>
       </c>
       <c r="E2">
         <f>SUMPRODUCT(Flatten!A2:A5, DenseParameters!E1:E4) + DenseParameters!E6</f>
-        <v>-2.3278629779815683</v>
+        <v>-0.27350366115570202</v>
       </c>
       <c r="F2">
         <f>SUMPRODUCT(Flatten!A2:A5, DenseParameters!F1:F4) + DenseParameters!F6</f>
-        <v>1.8645203113555908</v>
+        <v>-3.6052235066890717</v>
       </c>
       <c r="G2">
         <f>SUMPRODUCT(Flatten!A2:A5, DenseParameters!G1:G4) + DenseParameters!G6</f>
-        <v>9.2991260290145874</v>
+        <v>-0.88022840023040816</v>
       </c>
     </row>
   </sheetData>
@@ -1292,35 +1292,35 @@
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <f>EXP(Dense!A2)/($H$2)</f>
-        <v>1.8456526627206685E-4</v>
+        <v>1.6874997196870543E-2</v>
       </c>
       <c r="B2">
         <f>EXP(Dense!B2)/($H$2)</f>
-        <v>5.2293977437148446E-9</v>
+        <v>5.8759712017603083E-4</v>
       </c>
       <c r="C2">
         <f>EXP(Dense!C2)/($H$2)</f>
-        <v>3.5073681693775678E-2</v>
+        <v>2.0751469855564534E-2</v>
       </c>
       <c r="D2">
         <f>EXP(Dense!D2)/($H$2)</f>
-        <v>5.1897244285284601E-4</v>
+        <v>0.96054197833274124</v>
       </c>
       <c r="E2">
         <f>EXP(Dense!E2)/($H$2)</f>
-        <v>8.5976544740476487E-6</v>
+        <v>7.8688407498251256E-4</v>
       </c>
       <c r="F2">
         <f>EXP(Dense!F2)/($H$2)</f>
-        <v>5.6899561057757026E-4</v>
+        <v>2.8116626510902626E-5</v>
       </c>
       <c r="G2">
         <f>EXP(Dense!G2)/($H$2)</f>
-        <v>0.96364518210265004</v>
+        <v>4.2895679315429732E-4</v>
       </c>
       <c r="H2">
         <f>EXP(Dense!A2)+EXP(Dense!B2)+EXP(Dense!C2)+EXP(Dense!D2)+EXP(Dense!E2)+EXP(Dense!F2)+EXP(Dense!G2)</f>
-        <v>11340.754954063936</v>
+        <v>966.73649329040029</v>
       </c>
     </row>
   </sheetData>

</xml_diff>